<commit_message>
Analysis now supports 3 channels (FAM, VIC, ABY) and is agnostic to which channel is selected as reference. Analysis is performed on all channels if possible
</commit_message>
<xml_diff>
--- a/platemaps_template_blank.xlsx
+++ b/platemaps_template_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aviditybio-my.sharepoint.com/personal/aaron_aviditybio_com/Documents/Documents/Data/qPCR KD examples/2024-182 KD resources for automated in R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aviditybio-my.sharepoint.com/personal/aaron_aviditybio_com/Documents/Documents/R/qPCR-KD-excel-analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{92B9FA2F-FA20-49AE-B6C5-3FF83F21B849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E15456DE-C0FF-40FE-8E32-0992189222ED}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{92B9FA2F-FA20-49AE-B6C5-3FF83F21B849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C72FFC3D-C008-4AB3-9A05-19C449DAA7F6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFB4ECB9-805E-41A7-8DAD-80FD50BC8731}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FFB4ECB9-805E-41A7-8DAD-80FD50BC8731}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Design" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="51">
   <si>
     <r>
       <t xml:space="preserve">Fill out all tables in the </t>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Benchling Entity</t>
+  </si>
+  <si>
+    <t>ABY Probe</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -529,12 +532,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -544,26 +541,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -624,6 +613,19 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -638,36 +640,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89533663-FC49-4471-9F0E-FD5563AA0C5F}" name="StudyDesign_Benchling" displayName="StudyDesign_Benchling" ref="A1:S21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="20" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89533663-FC49-4471-9F0E-FD5563AA0C5F}" name="StudyDesign_Benchling" displayName="StudyDesign_Benchling" ref="A1:S21" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" dataCellStyle="Normal">
   <autoFilter ref="A1:S21" xr:uid="{89533663-FC49-4471-9F0E-FD5563AA0C5F}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{0DE663C8-A183-4207-9DD5-CA7E2DFDE974}" name="Entity" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{10240E5B-CAC2-4623-AEA5-75AF2EF008AC}" name="Group Number" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{26F992A1-EFEC-45CB-83F1-60B8EE840203}" name="Study" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{787BE4B9-9DE7-4036-85A9-FA173840B80D}" name="Treatment ID" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{25B5414D-044C-4916-A5BA-20FEA9BF596F}" name="Animal Strain" dataDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{27EA4B77-639B-4E88-8CB2-A1143389D346}" name="Number of Animals" dataDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{BE1B5633-B7EB-43F7-A276-1E4AA5817548}" name="Dose Material Type" dataDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{82BC3CBB-924F-41DF-BB80-16F2EA103722}" name="Dose Material" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{3ADC8C70-D84A-4A30-893C-98E3344605B8}" name="Number of Doses" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{F5FE4D6C-7282-41DC-B9C2-A09DC2D7F630}" name="Dose Schedule" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{85117B00-C37B-47B4-AA65-9B485515E383}" name="Survival Bleed Timepoints" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{42EF4C28-12E8-4AC6-BC0F-F11693CF1A8B}" name="Harvest (Day)" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="13" xr3:uid="{B433014E-72E2-4799-8FFD-1A1100E7C3CA}" name="Tissues/Fluids to Harvest" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="14" xr3:uid="{50A57464-8C8A-453D-8697-E11D552AA694}" name="Notes" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{E6FAE66A-D11C-4B35-9BC2-7003E563C814}" name="Dose Volume (mL/kg)" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="16" xr3:uid="{0B695120-7C21-42DD-88B5-D4A7475D2AA2}" name="Protein Dose Amount (mg/kg)" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="17" xr3:uid="{FBCCB91E-F260-4696-977D-664D60BD7AC7}" name="Oligo Dose Amount (mg/kg)" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="18" xr3:uid="{4DDD22A8-18FE-481E-8011-2ED144BC79E0}" name="Injection Volume per Animal (mL)" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="19" xr3:uid="{101C7AD6-6B90-4107-A87D-36334F00CAAB}" name="ROA" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{0DE663C8-A183-4207-9DD5-CA7E2DFDE974}" name="Entity" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{10240E5B-CAC2-4623-AEA5-75AF2EF008AC}" name="Group Number" dataDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{26F992A1-EFEC-45CB-83F1-60B8EE840203}" name="Study" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{787BE4B9-9DE7-4036-85A9-FA173840B80D}" name="Treatment ID" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{25B5414D-044C-4916-A5BA-20FEA9BF596F}" name="Animal Strain" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{27EA4B77-639B-4E88-8CB2-A1143389D346}" name="Number of Animals" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{BE1B5633-B7EB-43F7-A276-1E4AA5817548}" name="Dose Material Type" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{82BC3CBB-924F-41DF-BB80-16F2EA103722}" name="Dose Material" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{3ADC8C70-D84A-4A30-893C-98E3344605B8}" name="Number of Doses" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{F5FE4D6C-7282-41DC-B9C2-A09DC2D7F630}" name="Dose Schedule" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{85117B00-C37B-47B4-AA65-9B485515E383}" name="Survival Bleed Timepoints" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{42EF4C28-12E8-4AC6-BC0F-F11693CF1A8B}" name="Harvest (Day)" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{B433014E-72E2-4799-8FFD-1A1100E7C3CA}" name="Tissues/Fluids to Harvest" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="14" xr3:uid="{50A57464-8C8A-453D-8697-E11D552AA694}" name="Notes" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{E6FAE66A-D11C-4B35-9BC2-7003E563C814}" name="Dose Volume (mL/kg)" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="16" xr3:uid="{0B695120-7C21-42DD-88B5-D4A7475D2AA2}" name="Protein Dose Amount (mg/kg)" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="17" xr3:uid="{FBCCB91E-F260-4696-977D-664D60BD7AC7}" name="Oligo Dose Amount (mg/kg)" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="18" xr3:uid="{4DDD22A8-18FE-481E-8011-2ED144BC79E0}" name="Injection Volume per Animal (mL)" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="19" xr3:uid="{101C7AD6-6B90-4107-A87D-36334F00CAAB}" name="ROA" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F410A50-6CC1-43F1-B008-35DC38223848}" name="Probes_Benchling" displayName="Probes_Benchling" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{0F410A50-6CC1-43F1-B008-35DC38223848}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F410A50-6CC1-43F1-B008-35DC38223848}" name="Probes_Benchling" displayName="Probes_Benchling" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{0F410A50-6CC1-43F1-B008-35DC38223848}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{52DB729C-0401-4BD9-A136-9BC6830290A1}" name="Probe Assigned Name"/>
     <tableColumn id="2" xr3:uid="{1CB162B1-4FCD-48F8-9E14-FE6ACEDD4E7A}" name="Benchling Entity"/>
@@ -975,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C42458-E6C6-4C55-BE75-864B56C1A6CD}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -987,62 +989,62 @@
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="56" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:19" s="54" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="55" t="s">
+      <c r="N1" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="55" t="s">
+      <c r="O1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="55" t="s">
+      <c r="P1" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="Q1" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="S1" s="53" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1479,7 +1481,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,16 +1508,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3652441-68CB-4846-812E-E0D346D81F18}">
-  <dimension ref="A1:AA167"/>
+  <dimension ref="A1:AA185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="50" customWidth="1"/>
-    <col min="26" max="27" width="9.140625" style="57"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1549,32 +1550,32 @@
     </row>
     <row r="2" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
@@ -2788,32 +2789,32 @@
     </row>
     <row r="39" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1"/>
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="53"/>
-      <c r="S39" s="53"/>
-      <c r="T39" s="53"/>
-      <c r="U39" s="53"/>
-      <c r="V39" s="53"/>
-      <c r="W39" s="53"/>
-      <c r="X39" s="53"/>
-      <c r="Y39" s="53"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="56"/>
+      <c r="S39" s="56"/>
+      <c r="T39" s="56"/>
+      <c r="U39" s="56"/>
+      <c r="V39" s="56"/>
+      <c r="W39" s="56"/>
+      <c r="X39" s="56"/>
+      <c r="Y39" s="56"/>
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
     </row>
@@ -3423,32 +3424,32 @@
     </row>
     <row r="58" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="22"/>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="53"/>
-      <c r="M58" s="53"/>
-      <c r="N58" s="53"/>
-      <c r="O58" s="53"/>
-      <c r="P58" s="53"/>
-      <c r="Q58" s="53"/>
-      <c r="R58" s="53"/>
-      <c r="S58" s="53"/>
-      <c r="T58" s="53"/>
-      <c r="U58" s="53"/>
-      <c r="V58" s="53"/>
-      <c r="W58" s="53"/>
-      <c r="X58" s="53"/>
-      <c r="Y58" s="53"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="56"/>
+      <c r="N58" s="56"/>
+      <c r="O58" s="56"/>
+      <c r="P58" s="56"/>
+      <c r="Q58" s="56"/>
+      <c r="R58" s="56"/>
+      <c r="S58" s="56"/>
+      <c r="T58" s="56"/>
+      <c r="U58" s="56"/>
+      <c r="V58" s="56"/>
+      <c r="W58" s="56"/>
+      <c r="X58" s="56"/>
+      <c r="Y58" s="56"/>
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
     </row>
@@ -4662,32 +4663,32 @@
     </row>
     <row r="95" spans="1:27" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="22"/>
-      <c r="B95" s="52" t="s">
+      <c r="B95" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="52"/>
-      <c r="D95" s="52"/>
-      <c r="E95" s="52"/>
-      <c r="F95" s="52"/>
-      <c r="G95" s="52"/>
-      <c r="H95" s="52"/>
-      <c r="I95" s="52"/>
-      <c r="J95" s="52"/>
-      <c r="K95" s="52"/>
-      <c r="L95" s="52"/>
-      <c r="M95" s="52"/>
-      <c r="N95" s="52"/>
-      <c r="O95" s="52"/>
-      <c r="P95" s="52"/>
-      <c r="Q95" s="52"/>
-      <c r="R95" s="52"/>
-      <c r="S95" s="52"/>
-      <c r="T95" s="52"/>
-      <c r="U95" s="52"/>
-      <c r="V95" s="52"/>
-      <c r="W95" s="52"/>
-      <c r="X95" s="52"/>
-      <c r="Y95" s="52"/>
+      <c r="C95" s="55"/>
+      <c r="D95" s="55"/>
+      <c r="E95" s="55"/>
+      <c r="F95" s="55"/>
+      <c r="G95" s="55"/>
+      <c r="H95" s="55"/>
+      <c r="I95" s="55"/>
+      <c r="J95" s="55"/>
+      <c r="K95" s="55"/>
+      <c r="L95" s="55"/>
+      <c r="M95" s="55"/>
+      <c r="N95" s="55"/>
+      <c r="O95" s="55"/>
+      <c r="P95" s="55"/>
+      <c r="Q95" s="55"/>
+      <c r="R95" s="55"/>
+      <c r="S95" s="55"/>
+      <c r="T95" s="55"/>
+      <c r="U95" s="55"/>
+      <c r="V95" s="55"/>
+      <c r="W95" s="55"/>
+      <c r="X95" s="55"/>
+      <c r="Y95" s="55"/>
       <c r="Z95" s="2"/>
       <c r="AA95" s="2"/>
     </row>
@@ -7846,34 +7847,638 @@
       <c r="Z166" s="2"/>
       <c r="AA166" s="2"/>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
-      <c r="F167" s="2"/>
-      <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-      <c r="I167" s="2"/>
-      <c r="J167" s="2"/>
-      <c r="K167" s="2"/>
-      <c r="L167" s="2"/>
-      <c r="M167" s="2"/>
-      <c r="N167" s="2"/>
-      <c r="O167" s="2"/>
-      <c r="P167" s="2"/>
-      <c r="Q167" s="2"/>
-      <c r="R167" s="2"/>
-      <c r="S167" s="2"/>
-      <c r="T167" s="2"/>
-      <c r="U167" s="2"/>
-      <c r="V167" s="2"/>
-      <c r="W167" s="2"/>
-      <c r="X167" s="2"/>
-      <c r="Y167" s="2"/>
+    <row r="167" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="22"/>
+      <c r="B167" s="49"/>
+      <c r="C167" s="49"/>
+      <c r="D167" s="49"/>
+      <c r="E167" s="49"/>
+      <c r="F167" s="49"/>
+      <c r="G167" s="49"/>
+      <c r="H167" s="49"/>
+      <c r="I167" s="49"/>
+      <c r="J167" s="49"/>
+      <c r="K167" s="49"/>
+      <c r="L167" s="49"/>
+      <c r="M167" s="49"/>
+      <c r="N167" s="49"/>
+      <c r="O167" s="49"/>
+      <c r="P167" s="49"/>
+      <c r="Q167" s="49"/>
+      <c r="R167" s="49"/>
+      <c r="S167" s="49"/>
+      <c r="T167" s="49"/>
+      <c r="U167" s="49"/>
+      <c r="V167" s="49"/>
+      <c r="W167" s="49"/>
+      <c r="X167" s="49"/>
+      <c r="Y167" s="49"/>
       <c r="Z167" s="2"/>
       <c r="AA167" s="2"/>
+    </row>
+    <row r="168" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B168" s="34">
+        <v>1</v>
+      </c>
+      <c r="C168" s="34">
+        <v>2</v>
+      </c>
+      <c r="D168" s="34">
+        <v>3</v>
+      </c>
+      <c r="E168" s="34">
+        <v>4</v>
+      </c>
+      <c r="F168" s="34">
+        <v>5</v>
+      </c>
+      <c r="G168" s="34">
+        <v>6</v>
+      </c>
+      <c r="H168" s="34">
+        <v>7</v>
+      </c>
+      <c r="I168" s="34">
+        <v>8</v>
+      </c>
+      <c r="J168" s="34">
+        <v>9</v>
+      </c>
+      <c r="K168" s="34">
+        <v>10</v>
+      </c>
+      <c r="L168" s="34">
+        <v>11</v>
+      </c>
+      <c r="M168" s="34">
+        <v>12</v>
+      </c>
+      <c r="N168" s="34">
+        <v>13</v>
+      </c>
+      <c r="O168" s="34">
+        <v>14</v>
+      </c>
+      <c r="P168" s="34">
+        <v>15</v>
+      </c>
+      <c r="Q168" s="34">
+        <v>16</v>
+      </c>
+      <c r="R168" s="34">
+        <v>17</v>
+      </c>
+      <c r="S168" s="34">
+        <v>18</v>
+      </c>
+      <c r="T168" s="34">
+        <v>19</v>
+      </c>
+      <c r="U168" s="34">
+        <v>20</v>
+      </c>
+      <c r="V168" s="34">
+        <v>21</v>
+      </c>
+      <c r="W168" s="34">
+        <v>22</v>
+      </c>
+      <c r="X168" s="34">
+        <v>23</v>
+      </c>
+      <c r="Y168" s="35">
+        <v>24</v>
+      </c>
+      <c r="Z168" s="2"/>
+      <c r="AA168" s="2"/>
+    </row>
+    <row r="169" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A169" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B169" s="40"/>
+      <c r="C169" s="41"/>
+      <c r="D169" s="41"/>
+      <c r="E169" s="41"/>
+      <c r="F169" s="41"/>
+      <c r="G169" s="41"/>
+      <c r="H169" s="41"/>
+      <c r="I169" s="41"/>
+      <c r="J169" s="41"/>
+      <c r="K169" s="41"/>
+      <c r="L169" s="41"/>
+      <c r="M169" s="41"/>
+      <c r="N169" s="40"/>
+      <c r="O169" s="41"/>
+      <c r="P169" s="41"/>
+      <c r="Q169" s="41"/>
+      <c r="R169" s="41"/>
+      <c r="S169" s="41"/>
+      <c r="T169" s="41"/>
+      <c r="U169" s="41"/>
+      <c r="V169" s="41"/>
+      <c r="W169" s="41"/>
+      <c r="X169" s="41"/>
+      <c r="Y169" s="42"/>
+      <c r="Z169" s="2"/>
+      <c r="AA169" s="2"/>
+    </row>
+    <row r="170" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170" s="43"/>
+      <c r="C170" s="44"/>
+      <c r="D170" s="44"/>
+      <c r="E170" s="44"/>
+      <c r="F170" s="44"/>
+      <c r="G170" s="44"/>
+      <c r="H170" s="44"/>
+      <c r="I170" s="44"/>
+      <c r="J170" s="44"/>
+      <c r="K170" s="44"/>
+      <c r="L170" s="44"/>
+      <c r="M170" s="44"/>
+      <c r="N170" s="43"/>
+      <c r="O170" s="44"/>
+      <c r="P170" s="44"/>
+      <c r="Q170" s="44"/>
+      <c r="R170" s="44"/>
+      <c r="S170" s="44"/>
+      <c r="T170" s="44"/>
+      <c r="U170" s="44"/>
+      <c r="V170" s="44"/>
+      <c r="W170" s="44"/>
+      <c r="X170" s="44"/>
+      <c r="Y170" s="45"/>
+      <c r="Z170" s="2"/>
+      <c r="AA170" s="2"/>
+    </row>
+    <row r="171" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A171" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B171" s="43"/>
+      <c r="C171" s="44"/>
+      <c r="D171" s="44"/>
+      <c r="E171" s="44"/>
+      <c r="F171" s="44"/>
+      <c r="G171" s="44"/>
+      <c r="H171" s="44"/>
+      <c r="I171" s="44"/>
+      <c r="J171" s="44"/>
+      <c r="K171" s="44"/>
+      <c r="L171" s="44"/>
+      <c r="M171" s="44"/>
+      <c r="N171" s="43"/>
+      <c r="O171" s="44"/>
+      <c r="P171" s="44"/>
+      <c r="Q171" s="44"/>
+      <c r="R171" s="44"/>
+      <c r="S171" s="44"/>
+      <c r="T171" s="44"/>
+      <c r="U171" s="44"/>
+      <c r="V171" s="44"/>
+      <c r="W171" s="44"/>
+      <c r="X171" s="44"/>
+      <c r="Y171" s="45"/>
+      <c r="Z171" s="2"/>
+      <c r="AA171" s="2"/>
+    </row>
+    <row r="172" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A172" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" s="43"/>
+      <c r="C172" s="44"/>
+      <c r="D172" s="44"/>
+      <c r="E172" s="44"/>
+      <c r="F172" s="44"/>
+      <c r="G172" s="44"/>
+      <c r="H172" s="44"/>
+      <c r="I172" s="44"/>
+      <c r="J172" s="44"/>
+      <c r="K172" s="44"/>
+      <c r="L172" s="44"/>
+      <c r="M172" s="44"/>
+      <c r="N172" s="43"/>
+      <c r="O172" s="44"/>
+      <c r="P172" s="44"/>
+      <c r="Q172" s="44"/>
+      <c r="R172" s="44"/>
+      <c r="S172" s="44"/>
+      <c r="T172" s="44"/>
+      <c r="U172" s="44"/>
+      <c r="V172" s="44"/>
+      <c r="W172" s="44"/>
+      <c r="X172" s="44"/>
+      <c r="Y172" s="45"/>
+      <c r="Z172" s="2"/>
+      <c r="AA172" s="2"/>
+    </row>
+    <row r="173" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A173" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B173" s="43"/>
+      <c r="C173" s="44"/>
+      <c r="D173" s="44"/>
+      <c r="E173" s="44"/>
+      <c r="F173" s="44"/>
+      <c r="G173" s="44"/>
+      <c r="H173" s="44"/>
+      <c r="I173" s="44"/>
+      <c r="J173" s="44"/>
+      <c r="K173" s="44"/>
+      <c r="L173" s="44"/>
+      <c r="M173" s="44"/>
+      <c r="N173" s="43"/>
+      <c r="O173" s="44"/>
+      <c r="P173" s="44"/>
+      <c r="Q173" s="44"/>
+      <c r="R173" s="44"/>
+      <c r="S173" s="44"/>
+      <c r="T173" s="44"/>
+      <c r="U173" s="44"/>
+      <c r="V173" s="44"/>
+      <c r="W173" s="44"/>
+      <c r="X173" s="44"/>
+      <c r="Y173" s="45"/>
+      <c r="Z173" s="2"/>
+      <c r="AA173" s="2"/>
+    </row>
+    <row r="174" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A174" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B174" s="43"/>
+      <c r="C174" s="44"/>
+      <c r="D174" s="44"/>
+      <c r="E174" s="44"/>
+      <c r="F174" s="44"/>
+      <c r="G174" s="44"/>
+      <c r="H174" s="44"/>
+      <c r="I174" s="44"/>
+      <c r="J174" s="44"/>
+      <c r="K174" s="44"/>
+      <c r="L174" s="44"/>
+      <c r="M174" s="44"/>
+      <c r="N174" s="43"/>
+      <c r="O174" s="44"/>
+      <c r="P174" s="44"/>
+      <c r="Q174" s="44"/>
+      <c r="R174" s="44"/>
+      <c r="S174" s="44"/>
+      <c r="T174" s="44"/>
+      <c r="U174" s="44"/>
+      <c r="V174" s="44"/>
+      <c r="W174" s="44"/>
+      <c r="X174" s="44"/>
+      <c r="Y174" s="45"/>
+      <c r="Z174" s="2"/>
+      <c r="AA174" s="2"/>
+    </row>
+    <row r="175" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A175" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175" s="43"/>
+      <c r="C175" s="44"/>
+      <c r="D175" s="44"/>
+      <c r="E175" s="44"/>
+      <c r="F175" s="44"/>
+      <c r="G175" s="44"/>
+      <c r="H175" s="44"/>
+      <c r="I175" s="44"/>
+      <c r="J175" s="44"/>
+      <c r="K175" s="44"/>
+      <c r="L175" s="44"/>
+      <c r="M175" s="44"/>
+      <c r="N175" s="43"/>
+      <c r="O175" s="44"/>
+      <c r="P175" s="44"/>
+      <c r="Q175" s="44"/>
+      <c r="R175" s="44"/>
+      <c r="S175" s="44"/>
+      <c r="T175" s="44"/>
+      <c r="U175" s="44"/>
+      <c r="V175" s="44"/>
+      <c r="W175" s="44"/>
+      <c r="X175" s="44"/>
+      <c r="Y175" s="45"/>
+      <c r="Z175" s="2"/>
+      <c r="AA175" s="2"/>
+    </row>
+    <row r="176" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176" s="46"/>
+      <c r="C176" s="47"/>
+      <c r="D176" s="47"/>
+      <c r="E176" s="47"/>
+      <c r="F176" s="47"/>
+      <c r="G176" s="47"/>
+      <c r="H176" s="47"/>
+      <c r="I176" s="47"/>
+      <c r="J176" s="47"/>
+      <c r="K176" s="47"/>
+      <c r="L176" s="47"/>
+      <c r="M176" s="47"/>
+      <c r="N176" s="46"/>
+      <c r="O176" s="47"/>
+      <c r="P176" s="47"/>
+      <c r="Q176" s="47"/>
+      <c r="R176" s="47"/>
+      <c r="S176" s="47"/>
+      <c r="T176" s="47"/>
+      <c r="U176" s="47"/>
+      <c r="V176" s="47"/>
+      <c r="W176" s="47"/>
+      <c r="X176" s="47"/>
+      <c r="Y176" s="48"/>
+      <c r="Z176" s="2"/>
+      <c r="AA176" s="2"/>
+    </row>
+    <row r="177" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A177" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B177" s="43"/>
+      <c r="C177" s="44"/>
+      <c r="D177" s="44"/>
+      <c r="E177" s="44"/>
+      <c r="F177" s="44"/>
+      <c r="G177" s="44"/>
+      <c r="H177" s="44"/>
+      <c r="I177" s="44"/>
+      <c r="J177" s="44"/>
+      <c r="K177" s="44"/>
+      <c r="L177" s="44"/>
+      <c r="M177" s="44"/>
+      <c r="N177" s="43"/>
+      <c r="O177" s="44"/>
+      <c r="P177" s="44"/>
+      <c r="Q177" s="44"/>
+      <c r="R177" s="44"/>
+      <c r="S177" s="44"/>
+      <c r="T177" s="44"/>
+      <c r="U177" s="44"/>
+      <c r="V177" s="44"/>
+      <c r="W177" s="44"/>
+      <c r="X177" s="44"/>
+      <c r="Y177" s="45"/>
+      <c r="Z177" s="2"/>
+      <c r="AA177" s="2"/>
+    </row>
+    <row r="178" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A178" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B178" s="43"/>
+      <c r="C178" s="44"/>
+      <c r="D178" s="44"/>
+      <c r="E178" s="44"/>
+      <c r="F178" s="44"/>
+      <c r="G178" s="44"/>
+      <c r="H178" s="44"/>
+      <c r="I178" s="44"/>
+      <c r="J178" s="44"/>
+      <c r="K178" s="44"/>
+      <c r="L178" s="44"/>
+      <c r="M178" s="44"/>
+      <c r="N178" s="43"/>
+      <c r="O178" s="44"/>
+      <c r="P178" s="44"/>
+      <c r="Q178" s="44"/>
+      <c r="R178" s="44"/>
+      <c r="S178" s="44"/>
+      <c r="T178" s="44"/>
+      <c r="U178" s="44"/>
+      <c r="V178" s="44"/>
+      <c r="W178" s="44"/>
+      <c r="X178" s="44"/>
+      <c r="Y178" s="45"/>
+      <c r="Z178" s="2"/>
+      <c r="AA178" s="2"/>
+    </row>
+    <row r="179" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A179" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B179" s="43"/>
+      <c r="C179" s="44"/>
+      <c r="D179" s="44"/>
+      <c r="E179" s="44"/>
+      <c r="F179" s="44"/>
+      <c r="G179" s="44"/>
+      <c r="H179" s="44"/>
+      <c r="I179" s="44"/>
+      <c r="J179" s="44"/>
+      <c r="K179" s="44"/>
+      <c r="L179" s="44"/>
+      <c r="M179" s="44"/>
+      <c r="N179" s="43"/>
+      <c r="O179" s="44"/>
+      <c r="P179" s="44"/>
+      <c r="Q179" s="44"/>
+      <c r="R179" s="44"/>
+      <c r="S179" s="44"/>
+      <c r="T179" s="44"/>
+      <c r="U179" s="44"/>
+      <c r="V179" s="44"/>
+      <c r="W179" s="44"/>
+      <c r="X179" s="44"/>
+      <c r="Y179" s="45"/>
+      <c r="Z179" s="2"/>
+      <c r="AA179" s="2"/>
+    </row>
+    <row r="180" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A180" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B180" s="43"/>
+      <c r="C180" s="44"/>
+      <c r="D180" s="44"/>
+      <c r="E180" s="44"/>
+      <c r="F180" s="44"/>
+      <c r="G180" s="44"/>
+      <c r="H180" s="44"/>
+      <c r="I180" s="44"/>
+      <c r="J180" s="44"/>
+      <c r="K180" s="44"/>
+      <c r="L180" s="44"/>
+      <c r="M180" s="44"/>
+      <c r="N180" s="43"/>
+      <c r="O180" s="44"/>
+      <c r="P180" s="44"/>
+      <c r="Q180" s="44"/>
+      <c r="R180" s="44"/>
+      <c r="S180" s="44"/>
+      <c r="T180" s="44"/>
+      <c r="U180" s="44"/>
+      <c r="V180" s="44"/>
+      <c r="W180" s="44"/>
+      <c r="X180" s="44"/>
+      <c r="Y180" s="45"/>
+      <c r="Z180" s="2"/>
+      <c r="AA180" s="2"/>
+    </row>
+    <row r="181" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A181" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B181" s="43"/>
+      <c r="C181" s="44"/>
+      <c r="D181" s="44"/>
+      <c r="E181" s="44"/>
+      <c r="F181" s="44"/>
+      <c r="G181" s="44"/>
+      <c r="H181" s="44"/>
+      <c r="I181" s="44"/>
+      <c r="J181" s="44"/>
+      <c r="K181" s="44"/>
+      <c r="L181" s="44"/>
+      <c r="M181" s="44"/>
+      <c r="N181" s="43"/>
+      <c r="O181" s="44"/>
+      <c r="P181" s="44"/>
+      <c r="Q181" s="44"/>
+      <c r="R181" s="44"/>
+      <c r="S181" s="44"/>
+      <c r="T181" s="44"/>
+      <c r="U181" s="44"/>
+      <c r="V181" s="44"/>
+      <c r="W181" s="44"/>
+      <c r="X181" s="44"/>
+      <c r="Y181" s="45"/>
+      <c r="Z181" s="2"/>
+      <c r="AA181" s="2"/>
+    </row>
+    <row r="182" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A182" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B182" s="43"/>
+      <c r="C182" s="44"/>
+      <c r="D182" s="44"/>
+      <c r="E182" s="44"/>
+      <c r="F182" s="44"/>
+      <c r="G182" s="44"/>
+      <c r="H182" s="44"/>
+      <c r="I182" s="44"/>
+      <c r="J182" s="44"/>
+      <c r="K182" s="44"/>
+      <c r="L182" s="44"/>
+      <c r="M182" s="44"/>
+      <c r="N182" s="43"/>
+      <c r="O182" s="44"/>
+      <c r="P182" s="44"/>
+      <c r="Q182" s="44"/>
+      <c r="R182" s="44"/>
+      <c r="S182" s="44"/>
+      <c r="T182" s="44"/>
+      <c r="U182" s="44"/>
+      <c r="V182" s="44"/>
+      <c r="W182" s="44"/>
+      <c r="X182" s="44"/>
+      <c r="Y182" s="45"/>
+      <c r="Z182" s="2"/>
+      <c r="AA182" s="2"/>
+    </row>
+    <row r="183" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A183" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B183" s="43"/>
+      <c r="C183" s="44"/>
+      <c r="D183" s="44"/>
+      <c r="E183" s="44"/>
+      <c r="F183" s="44"/>
+      <c r="G183" s="44"/>
+      <c r="H183" s="44"/>
+      <c r="I183" s="44"/>
+      <c r="J183" s="44"/>
+      <c r="K183" s="44"/>
+      <c r="L183" s="44"/>
+      <c r="M183" s="44"/>
+      <c r="N183" s="43"/>
+      <c r="O183" s="44"/>
+      <c r="P183" s="44"/>
+      <c r="Q183" s="44"/>
+      <c r="R183" s="44"/>
+      <c r="S183" s="44"/>
+      <c r="T183" s="44"/>
+      <c r="U183" s="44"/>
+      <c r="V183" s="44"/>
+      <c r="W183" s="44"/>
+      <c r="X183" s="44"/>
+      <c r="Y183" s="45"/>
+      <c r="Z183" s="2"/>
+      <c r="AA183" s="2"/>
+    </row>
+    <row r="184" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B184" s="46"/>
+      <c r="C184" s="47"/>
+      <c r="D184" s="47"/>
+      <c r="E184" s="47"/>
+      <c r="F184" s="47"/>
+      <c r="G184" s="47"/>
+      <c r="H184" s="47"/>
+      <c r="I184" s="47"/>
+      <c r="J184" s="47"/>
+      <c r="K184" s="47"/>
+      <c r="L184" s="47"/>
+      <c r="M184" s="47"/>
+      <c r="N184" s="46"/>
+      <c r="O184" s="47"/>
+      <c r="P184" s="47"/>
+      <c r="Q184" s="47"/>
+      <c r="R184" s="47"/>
+      <c r="S184" s="47"/>
+      <c r="T184" s="47"/>
+      <c r="U184" s="47"/>
+      <c r="V184" s="47"/>
+      <c r="W184" s="47"/>
+      <c r="X184" s="47"/>
+      <c r="Y184" s="48"/>
+      <c r="Z184" s="2"/>
+      <c r="AA184" s="2"/>
+    </row>
+    <row r="185" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A185" s="1"/>
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
+      <c r="G185" s="2"/>
+      <c r="H185" s="2"/>
+      <c r="I185" s="2"/>
+      <c r="J185" s="2"/>
+      <c r="K185" s="2"/>
+      <c r="L185" s="2"/>
+      <c r="M185" s="2"/>
+      <c r="N185" s="2"/>
+      <c r="O185" s="2"/>
+      <c r="P185" s="2"/>
+      <c r="Q185" s="2"/>
+      <c r="R185" s="2"/>
+      <c r="S185" s="2"/>
+      <c r="T185" s="2"/>
+      <c r="U185" s="2"/>
+      <c r="V185" s="2"/>
+      <c r="W185" s="2"/>
+      <c r="X185" s="2"/>
+      <c r="Y185" s="2"/>
+      <c r="Z185" s="2"/>
+      <c r="AA185" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7883,7 +8488,7 @@
     <mergeCell ref="B95:Y95"/>
   </mergeCells>
   <conditionalFormatting sqref="B2">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7893,7 +8498,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7905,7 +8510,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7915,7 +8520,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7927,6 +8532,114 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:D29 H22:Y29 B30:Y37 B41:D48 H41:Y48 B49:Y56 B60:D67 H60:Y67 B68:Y76">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:M29">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:M37 B49:M56 B68:M76">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41:M48">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:M57 B58">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60:M67">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94:M94 B95">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:Y57 B58">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B78:Y93">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B86:Y93 B78:D85 H78:Y85">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -7938,7 +8651,55 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:M29">
+  <conditionalFormatting sqref="B94:Y94 B95">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B97:Y112">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B115:Y130">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B133:Y149 B151:Y166">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N22:Y29">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -7950,8 +8711,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:M37 B49:M56 B68:M76">
-    <cfRule type="colorScale" priority="53">
+  <conditionalFormatting sqref="N30:Y37 N49:Y56 N68:Y76">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7962,7 +8723,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41:M48">
+  <conditionalFormatting sqref="N32:Y37 N51:Y56 N70:Y76">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N41:Y48">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -7974,8 +8747,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57:M57 B58">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="N57:Y57">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7986,7 +8769,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B60:M67">
+  <conditionalFormatting sqref="N60:Y67">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -7998,8 +8781,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:M94 B95">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="N94:Y94">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -8009,8 +8792,6 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B57:Y57 B58">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -8022,172 +8803,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B78:Y93">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B86:Y93 B78:D85 H78:Y85">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B94:Y94 B95">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B97:Y112">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B115:Y130">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B133:Y149 B151:Y166">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22:Y29">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N30:Y37 N49:Y56 N68:Y76">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N32:Y37 N51:Y56 N70:Y76">
-    <cfRule type="colorScale" priority="55">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N41:Y48">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N57:Y57">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N60:Y67">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N94:Y94">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="B167:Y167 B169:Y184">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>